<commit_message>
Add a detected license column to the export report
</commit_message>
<xml_diff>
--- a/src/main/resources/template/OssList.xlsx
+++ b/src/main/resources/template/OssList.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\home\osc\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\fosslight_demo\src\main\resources\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60E38C61-DF0A-4D4F-80BB-DBE368A47820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7860"/>
+    <workbookView xWindow="-25410" yWindow="4065" windowWidth="21300" windowHeight="16050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,14 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>License Type</t>
   </si>
   <si>
-    <t>Obligation</t>
-  </si>
-  <si>
     <t>       </t>
   </si>
   <si>
@@ -45,9 +43,6 @@
   </si>
   <si>
     <t>Version</t>
-  </si>
-  <si>
-    <t>License</t>
   </si>
   <si>
     <t>Home Page</t>
@@ -68,13 +63,25 @@
   </si>
   <si>
     <t>Attribution</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Obligation</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> Detected License</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Declared License</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -183,7 +190,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -215,7 +222,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -493,11 +500,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -508,54 +515,57 @@
     <col min="5" max="5" width="17.625" customWidth="1"/>
     <col min="6" max="6" width="18.5" customWidth="1"/>
     <col min="7" max="7" width="15.375" customWidth="1"/>
-    <col min="8" max="8" width="15.875" customWidth="1"/>
-    <col min="9" max="9" width="28.5" customWidth="1"/>
-    <col min="10" max="12" width="30.5" customWidth="1"/>
-    <col min="13" max="13" width="14.25" customWidth="1"/>
+    <col min="8" max="9" width="15.875" customWidth="1"/>
+    <col min="10" max="10" width="28.5" customWidth="1"/>
+    <col min="11" max="13" width="30.5" customWidth="1"/>
+    <col min="14" max="14" width="14.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>4</v>
-      </c>
       <c r="F1" s="4" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="I1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>10</v>
-      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -569,8 +579,9 @@
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -579,8 +590,9 @@
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -589,16 +601,17 @@
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add search criteria to oss list
</commit_message>
<xml_diff>
--- a/src/main/resources/template/OssList.xlsx
+++ b/src/main/resources/template/OssList.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\fosslight_demo\src\main\resources\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60E38C61-DF0A-4D4F-80BB-DBE368A47820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25410" yWindow="4065" windowWidth="21300" windowHeight="16050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25416" yWindow="4068" windowWidth="21300" windowHeight="16056"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>License Type</t>
   </si>
@@ -75,13 +74,17 @@
   </si>
   <si>
     <t>Declared License</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Restriction</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -222,7 +225,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -500,28 +503,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="5.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="18.75" customWidth="1"/>
-    <col min="4" max="4" width="16.25" customWidth="1"/>
-    <col min="5" max="5" width="17.625" customWidth="1"/>
+    <col min="1" max="1" width="5.8984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="18.69921875" customWidth="1"/>
+    <col min="4" max="4" width="16.19921875" customWidth="1"/>
+    <col min="5" max="5" width="17.59765625" customWidth="1"/>
     <col min="6" max="6" width="18.5" customWidth="1"/>
-    <col min="7" max="7" width="15.375" customWidth="1"/>
-    <col min="8" max="9" width="15.875" customWidth="1"/>
-    <col min="10" max="10" width="28.5" customWidth="1"/>
-    <col min="11" max="13" width="30.5" customWidth="1"/>
-    <col min="14" max="14" width="14.25" customWidth="1"/>
+    <col min="7" max="8" width="15.3984375" customWidth="1"/>
+    <col min="9" max="10" width="15.8984375" customWidth="1"/>
+    <col min="11" max="11" width="28.5" customWidth="1"/>
+    <col min="12" max="14" width="30.5" customWidth="1"/>
+    <col min="15" max="15" width="14.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -544,28 +545,31 @@
         <v>0</v>
       </c>
       <c r="H1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -580,8 +584,9 @@
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" s="2"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -591,8 +596,9 @@
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" s="2"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -602,14 +608,15 @@
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>1</v>
       </c>

</xml_diff>